<commit_message>
Latest updates and data fixes. Need to add in strcuture for battery size improvements and for reductions in non-battery manufacturing costs.
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/FoTOMRAEL/Frac of Tech Outside Modeled Region Affecting Endo Learning.xlsx
+++ b/InputData/endo-learn/FoTOMRAEL/Frac of Tech Outside Modeled Region Affecting Endo Learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\FoTOMRAEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\endo-learn\FoTOMRAEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D1A431-AF32-4B88-8B24-231C99A9E877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D66D0B3-38C1-4094-A879-EA6D9F3F4DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -584,7 +584,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -604,7 +606,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5">
-        <v>0.25</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AEO updates - Endogenous learning for batteries
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/FoTOMRAEL/Frac of Tech Outside Modeled Region Affecting Endo Learning.xlsx
+++ b/InputData/endo-learn/FoTOMRAEL/Frac of Tech Outside Modeled Region Affecting Endo Learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\FoTOMRAEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\endo-learn\FoTOMRAEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D1A431-AF32-4B88-8B24-231C99A9E877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D66D0B3-38C1-4094-A879-EA6D9F3F4DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -584,7 +584,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -604,7 +606,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5">
-        <v>0.25</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use correct version of FoTOMRAEL from develop branch
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/FoTOMRAEL/Frac of Tech Outside Modeled Region Affecting Endo Learning.xlsx
+++ b/InputData/endo-learn/FoTOMRAEL/Frac of Tech Outside Modeled Region Affecting Endo Learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\endo-learn\FoTOMRAEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\FoTOMRAEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D66D0B3-38C1-4094-A879-EA6D9F3F4DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D1A431-AF32-4B88-8B24-231C99A9E877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -584,9 +584,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -606,7 +604,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5">
-        <v>0.9</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>